<commit_message>
Feb 2023 updates, expect this will need revision since branching now
- conversion to csv where possible
- updated some names to not use special symbols
- relaxed constraints so simulations starting in 2019 could use historical data
- adding regional data saving (China/RoW/Global)
- renamed a few functions to make more sense to not-John humans
- added code for getting q-values from p-values and estimating pi0
- updated case study data.xlsx, Price inputs.xlsx, price adjustment results.csv/xlsx with some new commodity data to enable Ta, W
</commit_message>
<xml_diff>
--- a/output_files/Historical tuning/2023-01-17 15_28_13_0_split_grades/input_files/Scenario setup.xlsx
+++ b/output_files/Historical tuning/2023-01-17 15_28_13_0_split_grades/input_files/Scenario setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/input_files/user_defined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495B843E-9DB7-864C-BF3C-E21B2A8664FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0073A8-6AC0-A24B-86EC-0001EF615DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12040" windowHeight="16080" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="312">
   <si>
     <t>Parameter category</t>
   </si>
@@ -68,9 +68,6 @@
     <t>volume_growth_rate</t>
   </si>
   <si>
-    <t>Commodity-specific</t>
-  </si>
-  <si>
     <t>Historical volume growth rate</t>
   </si>
   <si>
@@ -524,9 +521,6 @@
     <t>incentive_opening_probability</t>
   </si>
   <si>
-    <t>Fraction of profitable mines that are capable of opening that actually undergo opening, for any year</t>
-  </si>
-  <si>
     <t>[0.001,0.5]</t>
   </si>
   <si>
@@ -908,9 +902,6 @@
     <t>Standard deviation of product lifetime of sector - construction</t>
   </si>
   <si>
-    <t xml:space="preserve">Disclaimer on lifetime mean and standard deviation: we do not currently have it setup to dynamically change this value - changing it in 2003 would change how much scrap reaches end of life in 2003, as the lifetimes go into the cumulative density function determining this value directly, rather than setting the lifetime of products going forward. To get the desired effect, you would likely have to use a year farther in the future for the sector you are considering. This model is not stock driven, so changing lifetimes also will not change demand trajectories aside from the impacts the change in scrap generation has on prices and therefore demand. </t>
-  </si>
-  <si>
     <t>Variables that can be input as part of the giving your own mine set (other variables do exist and will be overwritten by combinations of these if given): ['Production fraction', 'Ramp up flag', 'Production (kt)', 'Region', 'Mine type', 'Mine type string', 'Risk indicator', 'Head grade (%)', 'Capacity utilization', 'Payable percent (%)', 'Recovery rate (%)', 'Reserves (kt)', 'Reserves (kt)', 'Cumulative ore treated ratio with ore treated', 'Cumulative ore treated (kt)', 'Opening', 'Initial ore treated (kt)', 'TCRC (USD/t)', 'Total cash margin (USD/t)', 'Minesite cost (USD/t)', 'Total cash cost (USD/t)', 'OGE', 'Sustaining CAPEX ($M)', 'Overhead ($M)', 'Total reclamation cost ($M)', 'Development CAPEX ($M)']</t>
   </si>
   <si>
@@ -969,13 +960,25 @@
   </si>
   <si>
     <t>If you would like to use real mine data rather than using statistically generated data, set this value to FALSE. For more information see the Notes tab of this spreadsheet.</t>
+  </si>
+  <si>
+    <t>Commodity-specific, based on real values</t>
+  </si>
+  <si>
+    <t>Fraction of profitable mines that are capable of opening that actually undergo opening, for any year. Zero represents a special case and should be avoided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Commodity Data values shown in gray have been given a default start year of 2001, since that is when the simulations technically begin. These values are changed upon simulation initialization, and cannot be changed unless some form of reinitialization takes place, which is not supported for the majority of these variables. Exceptions include fabrication efficiency and lifetime mean and standard deviation variables, though the disclaimer above still applies. Mining-related parameters also get reinitialized if you supply your own External mine file name (load_mine_file variable), so can be exceptions as well. Fabrication efficiencies </t>
+  </si>
+  <si>
+    <t>Disclaimer on fabrication efficiency and lifetime mean and standard deviation: we do not currently have it setup to dynamically change this value - changing it in 2003 would change how much scrap reaches end of life in 2003, as the lifetimes go into the cumulative density function determining this value directly, rather than setting the lifetime of products going forward. To get the desired effect, you would likely have to use a year farther in the future for the sector you are considering. This model is not stock driven, so changing lifetimes and fabrication efficiencies also will not change demand trajectories aside from the impacts the change in scrap generation has on prices and therefore demand. Fabrication efficiency changes will only impact the quantity of new scrap generated.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1007,6 +1010,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1028,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1043,6 +1061,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,8 +1094,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}" name="Table1" displayName="Table1" ref="A1:M95" totalsRowShown="0">
-  <autoFilter ref="A1:M95" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}" name="Table1" displayName="Table1" ref="A1:M96" totalsRowShown="0">
+  <autoFilter ref="A1:M96" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{C4332FCF-8E4C-4F49-8EFC-804C6E3A59B2}" name="Parameter category"/>
     <tableColumn id="2" xr3:uid="{A55A75DB-88A1-1245-BF1A-68A78F78C819}" name="Parameter name" dataDxfId="1"/>
@@ -1389,11 +1412,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70A1D66-ACB3-5F43-8146-4761D363CB09}">
-  <dimension ref="A1:M95"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1403,7 +1426,8 @@
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="89.5" customWidth="1"/>
     <col min="5" max="5" width="29.1640625" style="6" customWidth="1"/>
-    <col min="6" max="10" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="10" width="13.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -1423,19 +1447,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H1" t="s">
         <v>277</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>278</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>279</v>
-      </c>
-      <c r="I1" t="s">
-        <v>280</v>
-      </c>
-      <c r="J1" t="s">
-        <v>281</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -1444,585 +1468,594 @@
         <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>118</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>119</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>123</v>
       </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
         <v>125</v>
       </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
         <v>127</v>
       </c>
-      <c r="D5" t="s">
-        <v>128</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
         <v>129</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>130</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
         <v>133</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>134</v>
       </c>
-      <c r="D7" t="s">
-        <v>135</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" t="s">
         <v>136</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>137</v>
       </c>
-      <c r="D8" t="s">
-        <v>138</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" t="s">
         <v>139</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>140</v>
       </c>
-      <c r="D9" t="s">
-        <v>141</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" t="s">
         <v>142</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>143</v>
       </c>
-      <c r="D10" t="s">
-        <v>144</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" t="s">
         <v>145</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>146</v>
       </c>
-      <c r="D11" t="s">
-        <v>147</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" t="s">
         <v>148</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>149</v>
       </c>
-      <c r="D12" t="s">
-        <v>150</v>
-      </c>
       <c r="E12" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" t="s">
         <v>151</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>152</v>
       </c>
-      <c r="D13" t="s">
-        <v>153</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" t="s">
         <v>154</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>155</v>
       </c>
-      <c r="D14" t="s">
-        <v>156</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>158</v>
       </c>
-      <c r="D15" t="s">
-        <v>159</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" t="s">
         <v>160</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16">
+        <v>0.02</v>
+      </c>
+      <c r="K16">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" t="s">
+        <v>309</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17">
+        <v>0.03</v>
+      </c>
+      <c r="K17">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="C18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="D18" t="s">
         <v>164</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E18" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C19" t="s">
         <v>166</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="D19" t="s">
         <v>167</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E19" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="C20" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="D20" t="s">
         <v>171</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E20" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C21" t="s">
         <v>173</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="D21" t="s">
         <v>174</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E21" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C22" t="s">
         <v>176</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="D22" t="s">
         <v>177</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E22" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C23" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="D23" t="s">
         <v>180</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E23" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C24" t="s">
         <v>182</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="D24" t="s">
         <v>183</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E24" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="C25" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="D25" t="s">
         <v>187</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E25" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="C26" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="D26" t="s">
         <v>191</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E26" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="C27" t="s">
         <v>194</v>
       </c>
-      <c r="F25">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="D27" t="s">
         <v>195</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E27" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>196</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B28" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C28" t="s">
         <v>198</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="D28" t="s">
         <v>199</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E28" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C29" t="s">
         <v>201</v>
       </c>
-      <c r="E27" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>198</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="D29" t="s">
         <v>202</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E29" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C30" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="D30" t="s">
         <v>205</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E30" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="C31" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>198</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="D31" t="s">
         <v>209</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E31" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C32" t="s">
         <v>211</v>
       </c>
-      <c r="E30" s="6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>198</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="D32" t="s">
         <v>212</v>
       </c>
-      <c r="C31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D31" t="s">
-        <v>214</v>
-      </c>
-      <c r="E31" s="6">
+      <c r="E32" s="6">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>198</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C32" t="s">
-        <v>216</v>
-      </c>
-      <c r="D32" t="s">
-        <v>217</v>
-      </c>
-      <c r="E32" s="6">
-        <v>0.2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C33" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D33" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E33" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C34" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D34" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E34" s="6">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C35" t="s">
+        <v>220</v>
+      </c>
+      <c r="D35" t="s">
         <v>221</v>
-      </c>
-      <c r="C35" t="s">
-        <v>222</v>
-      </c>
-      <c r="D35" t="s">
-        <v>223</v>
       </c>
       <c r="E35" s="6">
         <v>0.4</v>
@@ -2030,16 +2063,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C36" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D36" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E36" s="6">
         <v>0.4</v>
@@ -2047,33 +2080,33 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C37" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D37" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E37" s="6">
-        <v>3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C38" t="s">
+        <v>226</v>
+      </c>
+      <c r="D38" t="s">
         <v>227</v>
-      </c>
-      <c r="C38" t="s">
-        <v>228</v>
-      </c>
-      <c r="D38" t="s">
-        <v>229</v>
       </c>
       <c r="E38" s="6">
         <v>3</v>
@@ -2081,50 +2114,50 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C39" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D39" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E39" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D40" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E40" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C41" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E41" s="6">
         <v>10</v>
@@ -2132,908 +2165,1465 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C42" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D42" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E42" s="6">
-        <v>0.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C43" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D43" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E43" s="6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C44" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D44" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E44" s="6">
-        <v>20220208</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C45" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D45" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E45" s="6">
-        <v>0.95</v>
+        <v>20220208</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>304</v>
+        <v>250</v>
       </c>
       <c r="C46" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="D46" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
       <c r="E46" s="6">
-        <v>20</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C47" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="D47" t="s">
-        <v>310</v>
-      </c>
-      <c r="E47" s="6" t="b">
-        <v>1</v>
+        <v>304</v>
+      </c>
+      <c r="E47" s="6">
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C48" t="s">
+        <v>292</v>
+      </c>
+      <c r="D48" t="s">
+        <v>307</v>
+      </c>
+      <c r="E48" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C49" t="s">
+        <v>293</v>
+      </c>
+      <c r="D49" t="s">
+        <v>306</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C48" t="s">
-        <v>296</v>
-      </c>
-      <c r="D48" t="s">
-        <v>309</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>256</v>
-      </c>
-      <c r="B49" s="1" t="s">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>254</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C50" t="s">
+        <v>241</v>
+      </c>
+      <c r="D50" t="s">
         <v>242</v>
-      </c>
-      <c r="C49" t="s">
-        <v>243</v>
-      </c>
-      <c r="D49" t="s">
-        <v>244</v>
-      </c>
-      <c r="E49" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>256</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C50" t="s">
-        <v>269</v>
-      </c>
-      <c r="D50" t="s">
-        <v>245</v>
       </c>
       <c r="E50" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>254</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" t="s">
+        <v>267</v>
+      </c>
+      <c r="D51" t="s">
+        <v>243</v>
+      </c>
+      <c r="E51" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>254</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C52" t="s">
+        <v>255</v>
+      </c>
+      <c r="D52" t="s">
+        <v>273</v>
+      </c>
+      <c r="E52" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>254</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C53" t="s">
         <v>256</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C51" t="s">
-        <v>257</v>
-      </c>
-      <c r="D51" t="s">
-        <v>275</v>
-      </c>
-      <c r="E51" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>256</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C52" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" t="s">
-        <v>276</v>
-      </c>
-      <c r="E52" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>256</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C53" t="s">
-        <v>259</v>
+      <c r="D53" t="s">
+        <v>274</v>
       </c>
       <c r="E53" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C54" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E54" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>264</v>
       </c>
       <c r="C55" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C56" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="E56" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>8</v>
+        <v>263</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E57" s="6">
-        <v>2.546855E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>281</v>
+      </c>
+      <c r="E58" s="6">
+        <v>2.546855E-2</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D59" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E59" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L59" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M59" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="C60" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L60" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M60" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="B61" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="C61" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L61" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M61" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="B62" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="C62" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L62" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M62" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B63" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="C63" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L63" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M63" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="B64" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="C64" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L64" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M64" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" t="s">
-        <v>27</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B65" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="C65" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L65" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M65" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="B66" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E64" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="C66" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L66" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M66" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" t="s">
-        <v>33</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="B67" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E65" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="C67" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L67" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M67" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C66" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="B68" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E66" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="C68" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L68" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M68" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="B69" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E67" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="C69" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L69" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M69" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="B70" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E68" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="C70" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L70" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M70" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C69" t="s">
-        <v>45</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="B71" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="C71" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L71" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M71" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A72" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C70" t="s">
-        <v>48</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="B72" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E70" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="C72" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L72" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M72" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C71" t="s">
-        <v>51</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="B73" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E71" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="C73" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L73" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M73" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C72" t="s">
-        <v>54</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="B74" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E72" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="C74" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L74" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M74" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C73" t="s">
-        <v>57</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="B75" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E73" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="C75" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L75" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M75" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B76" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D74" t="s">
+      <c r="C76" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L76" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M76" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E74" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="E77" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L77" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M77" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="B78" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D78" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="E75" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="E78" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L78" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M78" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C76" t="s">
-        <v>64</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="B79" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="E76" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="E79" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L79" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M79" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" t="s">
-        <v>66</v>
-      </c>
-      <c r="D77" t="s">
-        <v>288</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="B80" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L80" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M80" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C78" t="s">
-        <v>68</v>
-      </c>
-      <c r="D78" t="s">
-        <v>289</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="B81" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L81" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M81" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C79" t="s">
-        <v>70</v>
-      </c>
-      <c r="D79" t="s">
-        <v>71</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="B82" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="7"/>
+      <c r="K82" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L82" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M82" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C80" t="s">
-        <v>73</v>
-      </c>
-      <c r="D80" t="s">
-        <v>74</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="B83" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L83" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M83" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C81" t="s">
-        <v>76</v>
-      </c>
-      <c r="D81" t="s">
-        <v>77</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="B84" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="7"/>
+      <c r="K84" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L84" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M84" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C82" t="s">
-        <v>79</v>
-      </c>
-      <c r="D82" t="s">
-        <v>80</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="B85" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L85" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M85" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" t="s">
-        <v>82</v>
-      </c>
-      <c r="D83" t="s">
-        <v>83</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="B86" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L86" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M86" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C84" t="s">
-        <v>84</v>
-      </c>
-      <c r="D84" t="s">
-        <v>85</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="B87" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L87" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M87" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A88" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C85" t="s">
-        <v>86</v>
-      </c>
-      <c r="D85" t="s">
-        <v>87</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="B88" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="7"/>
+      <c r="K88" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L88" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M88" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C86" t="s">
-        <v>89</v>
-      </c>
-      <c r="D86" t="s">
-        <v>90</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="B89" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+      <c r="I89" s="7"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L89" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M89" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="B90" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D90" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D87" t="s">
-        <v>93</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="E90" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L90" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M90" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C88" t="s">
-        <v>95</v>
-      </c>
-      <c r="D88" t="s">
-        <v>96</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="B91" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L91" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M91" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" t="s">
-        <v>98</v>
-      </c>
-      <c r="D89" t="s">
-        <v>93</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="B92" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="7"/>
+      <c r="K92" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L92" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M92" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D90" t="s">
-        <v>101</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="B93" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L93" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M93" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C91" t="s">
-        <v>103</v>
-      </c>
-      <c r="D91" t="s">
-        <v>104</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="B94" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L94" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M94" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C92" t="s">
-        <v>106</v>
-      </c>
-      <c r="D92" t="s">
-        <v>107</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="B95" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="7"/>
+      <c r="I95" s="7"/>
+      <c r="J95" s="7"/>
+      <c r="K95" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L95" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M95" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C93" t="s">
-        <v>109</v>
-      </c>
-      <c r="D93" t="s">
-        <v>110</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C94" t="s">
-        <v>112</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="B96" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E94" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>7</v>
-      </c>
-      <c r="B95" s="1" t="s">
+      <c r="C96" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D96" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D95" t="s">
-        <v>116</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>10</v>
+      <c r="E96" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7"/>
+      <c r="J96" s="7"/>
+      <c r="K96" s="7">
+        <v>2001</v>
+      </c>
+      <c r="L96" s="7">
+        <v>2001</v>
+      </c>
+      <c r="M96" s="7">
+        <v>2001</v>
       </c>
     </row>
   </sheetData>
@@ -3047,10 +3637,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD35743A-9BCD-4440-A2B9-C15CACDD5C34}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3060,20 +3650,20 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="N1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="44" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3091,7 +3681,7 @@
     </row>
     <row r="4" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -3109,7 +3699,7 @@
     </row>
     <row r="5" spans="1:14" ht="22" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3127,7 +3717,7 @@
     </row>
     <row r="6" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3145,7 +3735,7 @@
     </row>
     <row r="7" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3163,7 +3753,7 @@
     </row>
     <row r="8" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3179,9 +3769,9 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="132" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3197,8 +3787,10 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>310</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3213,10 +3805,8 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="22" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>298</v>
-      </c>
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3231,9 +3821,9 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="132" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>297</v>
+    <row r="12" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3249,9 +3839,9 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="88" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="132" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3267,9 +3857,9 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="88" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3285,9 +3875,9 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="132" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="110" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3303,8 +3893,10 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:14" ht="132" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>297</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -3319,10 +3911,8 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="22" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>299</v>
-      </c>
+    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -3337,9 +3927,9 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="88" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>301</v>
+    <row r="18" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3355,8 +3945,10 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:14" ht="88" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -3483,6 +4075,22 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
+    <row r="27" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>